<commit_message>
Finished editing HTML readme.
</commit_message>
<xml_diff>
--- a/SIMS_PCA/SIMS_PCA/sims-data/OriginalData/Grouping List.xlsx
+++ b/SIMS_PCA/SIMS_PCA/sims-data/OriginalData/Grouping List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\cswelch\pca\SIMS_PCA\SIMS_PCA\sims-data\OriginalData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175747F2-CCF5-419D-8DC0-659444A4BA3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B004C247-AD9E-4C45-8755-24A69CFD0F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1221,7 +1221,7 @@
   <dimension ref="A1:I207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
Updated metadata.txt for new data and updated plotting code to handle the more flexible labeling conventions required. Still getting a divide by 0 error somewhere.
</commit_message>
<xml_diff>
--- a/SIMS_PCA/SIMS_PCA/sims-data/OriginalData/Grouping List.xlsx
+++ b/SIMS_PCA/SIMS_PCA/sims-data/OriginalData/Grouping List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\cswelch\pca\SIMS_PCA\SIMS_PCA\sims-data\OriginalData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B004C247-AD9E-4C45-8755-24A69CFD0F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0262458A-28CB-42D4-9425-B7E3AEA42EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1220,8 +1220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E86B7E7-C1C0-1847-A1E7-E8079898BAB8}">
   <dimension ref="A1:I207"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>

</xml_diff>